<commit_message>
Added new info on test subject + new scores.
</commit_message>
<xml_diff>
--- a/R_Analysis/DATA COLLECTION STATS.xlsx
+++ b/R_Analysis/DATA COLLECTION STATS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
   <si>
     <t xml:space="preserve">Last Name </t>
   </si>
@@ -154,6 +154,42 @@
   </si>
   <si>
     <t>Leung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambrosino </t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Test 8 pas 1</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>test 1 pas 1</t>
+  </si>
+  <si>
+    <t>Alexis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female </t>
+  </si>
+  <si>
+    <t>Test 8 pas 2</t>
+  </si>
+  <si>
+    <t>Sasanuma</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>test 3 pas 1</t>
   </si>
 </sst>
 </file>
@@ -209,8 +245,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -222,11 +266,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -650,85 +702,85 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2">
+        <v>20170429</v>
+      </c>
+      <c r="H3" s="2">
+        <v>150154</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7</v>
+      </c>
+      <c r="K3" s="2">
+        <v>4</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>20170430</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>144237</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <v>7</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2">
-        <v>20170429</v>
-      </c>
-      <c r="H4" s="2">
-        <v>150154</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2">
-        <v>7</v>
-      </c>
-      <c r="K4" s="2">
-        <v>4</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>11</v>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1057,6 +1109,293 @@
       </c>
       <c r="M12">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13">
+        <v>20170617</v>
+      </c>
+      <c r="H13">
+        <v>170926</v>
+      </c>
+      <c r="I13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14">
+        <v>20170617</v>
+      </c>
+      <c r="H14">
+        <v>192567</v>
+      </c>
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15">
+        <v>20170617</v>
+      </c>
+      <c r="H15">
+        <v>174536</v>
+      </c>
+      <c r="I15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16">
+        <v>20170617</v>
+      </c>
+      <c r="H16">
+        <v>175545</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>20170619</v>
+      </c>
+      <c r="H17">
+        <v>174323</v>
+      </c>
+      <c r="I17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>20170619</v>
+      </c>
+      <c r="H18">
+        <v>175643</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19">
+        <v>20170624</v>
+      </c>
+      <c r="H19">
+        <v>174536</v>
+      </c>
+      <c r="I19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the time ID in excel file and Bad data column
</commit_message>
<xml_diff>
--- a/R_Analysis/DATA COLLECTION STATS.xlsx
+++ b/R_Analysis/DATA COLLECTION STATS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\EyeTribeDataCollection\R_Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
-  <si>
-    <t xml:space="preserve">Last Name </t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>Age</t>
   </si>
@@ -39,15 +38,6 @@
     <t>Nationality</t>
   </si>
   <si>
-    <t xml:space="preserve">Date of Experiment </t>
-  </si>
-  <si>
-    <t>Time of Experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Passage Title </t>
-  </si>
-  <si>
     <t>Howe</t>
   </si>
   <si>
@@ -66,18 +56,6 @@
     <t>This passage is from Charlotte Brontë, The Professor, originally published in 1857.</t>
   </si>
   <si>
-    <t>Correct Answer</t>
-  </si>
-  <si>
-    <t>Incorrect Answer</t>
-  </si>
-  <si>
-    <t>No Answer</t>
-  </si>
-  <si>
-    <t>Total Questions</t>
-  </si>
-  <si>
     <t>Kraft</t>
   </si>
   <si>
@@ -190,6 +168,36 @@
   </si>
   <si>
     <t>test 3 pas 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last_Name </t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Time_of_Experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date_of_Experiment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passage_Title </t>
+  </si>
+  <si>
+    <t>Correct_Answer</t>
+  </si>
+  <si>
+    <t>Incorrect_Answer</t>
+  </si>
+  <si>
+    <t>No_Answer</t>
+  </si>
+  <si>
+    <t>Total_Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad_Data </t>
   </si>
 </sst>
 </file>
@@ -283,6 +291,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -608,85 +624,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>20170429</v>
       </c>
       <c r="H2">
-        <v>160000</v>
+        <v>160122</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1">
         <v>6</v>
@@ -700,34 +719,37 @@
       <c r="M2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2">
         <v>20170429</v>
       </c>
       <c r="H3" s="2">
-        <v>150154</v>
+        <v>150255</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J3" s="2">
         <v>7</v>
@@ -741,34 +763,37 @@
       <c r="M3" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
       </c>
       <c r="G4">
         <v>20170430</v>
       </c>
       <c r="H4">
-        <v>144237</v>
+        <v>143937</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J4">
         <v>7</v>
@@ -782,34 +807,37 @@
       <c r="M4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G5">
         <v>20170603</v>
       </c>
       <c r="H5">
-        <v>185903</v>
+        <v>185654</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="J5">
         <v>10</v>
@@ -823,34 +851,37 @@
       <c r="M5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>20170603</v>
       </c>
       <c r="H6">
-        <v>191032</v>
+        <v>191010</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J6">
         <v>8</v>
@@ -864,34 +895,37 @@
       <c r="M6">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G7">
         <v>20170603</v>
       </c>
       <c r="H7">
-        <v>193305</v>
+        <v>193919</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J7">
         <v>9</v>
@@ -905,34 +939,37 @@
       <c r="M7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G8">
         <v>20170603</v>
       </c>
       <c r="H8">
-        <v>194934</v>
+        <v>194937</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J8">
         <v>8</v>
@@ -946,34 +983,37 @@
       <c r="M8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G9">
         <v>20170609</v>
       </c>
       <c r="H9">
-        <v>193550</v>
+        <v>192957</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="J9">
         <v>9</v>
@@ -987,34 +1027,37 @@
       <c r="M9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G10">
         <v>20170609</v>
       </c>
       <c r="H10">
-        <v>194534</v>
+        <v>194603</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J10">
         <v>11</v>
@@ -1028,34 +1071,37 @@
       <c r="M10">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G11">
         <v>20170609</v>
       </c>
       <c r="H11">
-        <v>202921</v>
+        <v>202514</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="J11">
         <v>7</v>
@@ -1069,34 +1115,37 @@
       <c r="M11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G12">
         <v>20170609</v>
       </c>
       <c r="H12">
-        <v>204556</v>
+        <v>204405</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J12">
         <v>9</v>
@@ -1110,34 +1159,37 @@
       <c r="M12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G13">
         <v>20170617</v>
       </c>
       <c r="H13">
-        <v>170926</v>
+        <v>170520</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J13">
         <v>10</v>
@@ -1151,34 +1203,37 @@
       <c r="M13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G14">
         <v>20170617</v>
       </c>
       <c r="H14">
-        <v>192567</v>
+        <v>192040</v>
       </c>
       <c r="I14" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J14">
         <v>10</v>
@@ -1192,34 +1247,37 @@
       <c r="M14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
         <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
       </c>
       <c r="G15">
         <v>20170617</v>
       </c>
       <c r="H15">
-        <v>174536</v>
+        <v>175032</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="J15">
         <v>9</v>
@@ -1233,34 +1291,37 @@
       <c r="M15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
         <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
       </c>
       <c r="G16">
         <v>20170617</v>
       </c>
       <c r="H16">
-        <v>175545</v>
+        <v>175948</v>
       </c>
       <c r="I16" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J16">
         <v>10</v>
@@ -1274,34 +1335,37 @@
       <c r="M16">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C17">
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G17">
         <v>20170619</v>
       </c>
       <c r="H17">
-        <v>174323</v>
+        <v>180053</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="J17">
         <v>10</v>
@@ -1315,34 +1379,37 @@
       <c r="M17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>20170619</v>
       </c>
       <c r="H18">
-        <v>175643</v>
+        <v>181931</v>
       </c>
       <c r="I18" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J18">
         <v>11</v>
@@ -1356,34 +1423,37 @@
       <c r="M18">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
         <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>21</v>
       </c>
       <c r="G19">
         <v>20170624</v>
       </c>
       <c r="H19">
-        <v>174536</v>
+        <v>190525</v>
       </c>
       <c r="I19" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="J19">
         <v>8</v>
@@ -1396,6 +1466,9 @@
       </c>
       <c r="M19">
         <v>10</v>
+      </c>
+      <c r="N19" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correlation Analysis (Not Done yet)
</commit_message>
<xml_diff>
--- a/R_Analysis/DATA COLLECTION STATS.xlsx
+++ b/R_Analysis/DATA COLLECTION STATS.xlsx
@@ -164,9 +164,6 @@
     <t>Sasanuma</t>
   </si>
   <si>
-    <t>Chris</t>
-  </si>
-  <si>
     <t>test 3 pas 1</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bad_Data </t>
+  </si>
+  <si>
+    <t>Christopher</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -637,10 +637,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -655,28 +655,28 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>54</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>56</v>
-      </c>
-      <c r="N1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="2">
-        <v>20170429</v>
+        <v>20170430</v>
       </c>
       <c r="H3" s="2">
         <v>150255</v>
@@ -831,7 +831,7 @@
         <v>19</v>
       </c>
       <c r="G5">
-        <v>20170603</v>
+        <v>20170503</v>
       </c>
       <c r="H5">
         <v>185654</v>
@@ -875,7 +875,7 @@
         <v>20</v>
       </c>
       <c r="G6">
-        <v>20170603</v>
+        <v>20170503</v>
       </c>
       <c r="H6">
         <v>191010</v>
@@ -919,7 +919,7 @@
         <v>23</v>
       </c>
       <c r="G7">
-        <v>20170603</v>
+        <v>20170503</v>
       </c>
       <c r="H7">
         <v>193919</v>
@@ -963,7 +963,7 @@
         <v>23</v>
       </c>
       <c r="G8">
-        <v>20170603</v>
+        <v>20170503</v>
       </c>
       <c r="H8">
         <v>194937</v>
@@ -1007,7 +1007,7 @@
         <v>29</v>
       </c>
       <c r="G9">
-        <v>20170609</v>
+        <v>20170509</v>
       </c>
       <c r="H9">
         <v>192957</v>
@@ -1051,7 +1051,7 @@
         <v>29</v>
       </c>
       <c r="G10">
-        <v>20170609</v>
+        <v>20170509</v>
       </c>
       <c r="H10">
         <v>194603</v>
@@ -1095,7 +1095,7 @@
         <v>32</v>
       </c>
       <c r="G11">
-        <v>20170609</v>
+        <v>20170509</v>
       </c>
       <c r="H11">
         <v>202514</v>
@@ -1139,7 +1139,7 @@
         <v>32</v>
       </c>
       <c r="G12">
-        <v>20170609</v>
+        <v>20170509</v>
       </c>
       <c r="H12">
         <v>204405</v>
@@ -1183,7 +1183,7 @@
         <v>23</v>
       </c>
       <c r="G13">
-        <v>20170617</v>
+        <v>20170517</v>
       </c>
       <c r="H13">
         <v>170520</v>
@@ -1227,7 +1227,7 @@
         <v>23</v>
       </c>
       <c r="G14">
-        <v>20170617</v>
+        <v>20170517</v>
       </c>
       <c r="H14">
         <v>192040</v>
@@ -1271,7 +1271,7 @@
         <v>12</v>
       </c>
       <c r="G15">
-        <v>20170617</v>
+        <v>20170517</v>
       </c>
       <c r="H15">
         <v>175032</v>
@@ -1315,7 +1315,7 @@
         <v>12</v>
       </c>
       <c r="G16">
-        <v>20170617</v>
+        <v>20170517</v>
       </c>
       <c r="H16">
         <v>175948</v>
@@ -1359,7 +1359,7 @@
         <v>8</v>
       </c>
       <c r="G17">
-        <v>20170619</v>
+        <v>20170519</v>
       </c>
       <c r="H17">
         <v>180053</v>
@@ -1403,7 +1403,7 @@
         <v>8</v>
       </c>
       <c r="G18">
-        <v>20170619</v>
+        <v>20170519</v>
       </c>
       <c r="H18">
         <v>181931</v>
@@ -1432,7 +1432,7 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C19">
         <v>16</v>
@@ -1447,13 +1447,13 @@
         <v>12</v>
       </c>
       <c r="G19">
-        <v>20170624</v>
+        <v>20170525</v>
       </c>
       <c r="H19">
         <v>190525</v>
       </c>
       <c r="I19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19">
         <v>8</v>

</xml_diff>